<commit_message>
finishing upload excel for anggota cu
</commit_message>
<xml_diff>
--- a/public/files/formatAnggotaCu.xlsx
+++ b/public/files/formatAnggotaCu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Sites/bkcuvue/public/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BE48BD-C237-C54D-95BC-005ED6BCA2BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4183DDE3-4052-3149-9A4D-10E0B5AEE296}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="460" windowWidth="27320" windowHeight="14900" xr2:uid="{6E3E5F2B-8BA1-F845-BBF4-F30D4ACC6EF2}"/>
+    <workbookView xWindow="740" yWindow="1780" windowWidth="27320" windowHeight="14900" xr2:uid="{6E3E5F2B-8BA1-F845-BBF4-F30D4ACC6EF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -234,9 +234,6 @@
     <t>Manumuti</t>
   </si>
   <si>
-    <t>Laki-Laki</t>
-  </si>
-  <si>
     <t>Nifuboke</t>
   </si>
   <si>
@@ -496,6 +493,9 @@
   </si>
   <si>
     <t>sss</t>
+  </si>
+  <si>
+    <t>pria</t>
   </si>
 </sst>
 </file>
@@ -943,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B728F6F-ED4D-754B-AFD8-5624DAAEA7F5}">
   <dimension ref="A1:AF12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="239" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="239" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1081,13 +1081,13 @@
         <v>26751</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>42</v>
+        <v>129</v>
       </c>
       <c r="J2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="L2" s="7">
         <v>1</v>
@@ -1096,31 +1096,31 @@
         <v>1</v>
       </c>
       <c r="O2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="S2" s="10">
         <v>40265</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="X2">
         <v>200000</v>
@@ -1129,25 +1129,25 @@
         <v>100000</v>
       </c>
       <c r="Z2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AA2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AB2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AC2">
         <v>150</v>
       </c>
       <c r="AD2" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AE2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AF2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.2">
@@ -1170,16 +1170,16 @@
         <v>353453453</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H3" s="5">
         <v>24028</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>42</v>
+        <v>129</v>
       </c>
       <c r="J3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K3" s="8"/>
       <c r="L3" s="7">
@@ -1189,31 +1189,31 @@
         <v>3</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="Q3" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="R3" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S3" s="10">
         <v>40266</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="X3">
         <v>200000</v>
@@ -1222,25 +1222,25 @@
         <v>100000</v>
       </c>
       <c r="Z3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AA3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AB3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AC3">
         <v>155</v>
       </c>
       <c r="AD3" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AE3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
@@ -1257,22 +1257,22 @@
         <v>34</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F4">
         <v>435345435</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4" s="5">
         <v>29596</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>42</v>
+        <v>129</v>
       </c>
       <c r="J4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K4" s="8"/>
       <c r="L4" s="7">
@@ -1282,31 +1282,31 @@
         <v>1</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="Q4" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="R4" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S4" s="10">
         <v>40267</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="X4">
         <v>230000</v>
@@ -1315,25 +1315,25 @@
         <v>80000</v>
       </c>
       <c r="Z4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AA4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AB4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AC4">
         <v>150</v>
       </c>
       <c r="AD4" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AE4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AF4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.2">
@@ -1350,22 +1350,22 @@
         <v>35</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F5">
         <v>233333333</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H5" s="5">
         <v>28295</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>42</v>
+        <v>129</v>
       </c>
       <c r="J5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K5" s="8"/>
       <c r="L5" s="7">
@@ -1375,31 +1375,31 @@
         <v>1</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="Q5" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="R5" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S5" s="10">
         <v>40268</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="V5" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W5" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="X5">
         <v>500000</v>
@@ -1408,25 +1408,25 @@
         <v>400000</v>
       </c>
       <c r="Z5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AA5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AB5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AC5">
         <v>160</v>
       </c>
       <c r="AD5" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AE5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.2">
@@ -1443,22 +1443,22 @@
         <v>36</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F6">
         <v>432432423</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H6" s="5">
         <v>29529</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>42</v>
+        <v>129</v>
       </c>
       <c r="J6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K6" s="8"/>
       <c r="L6" s="7">
@@ -1468,31 +1468,31 @@
         <v>1</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="Q6" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="R6" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="S6" s="10">
         <v>40269</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V6" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W6" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="X6">
         <v>1000000</v>
@@ -1501,25 +1501,25 @@
         <v>400000</v>
       </c>
       <c r="Z6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AB6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AC6">
         <v>150</v>
       </c>
       <c r="AD6" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AE6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.2">
@@ -1536,22 +1536,22 @@
         <v>37</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F7">
         <v>342423423</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H7" s="5">
         <v>31010</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>42</v>
+        <v>129</v>
       </c>
       <c r="J7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K7" s="8"/>
       <c r="L7" s="7">
@@ -1561,31 +1561,31 @@
         <v>1</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="Q7" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="R7" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S7" s="10">
         <v>40270</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="V7" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="X7">
         <v>1200000</v>
@@ -1594,25 +1594,25 @@
         <v>500000</v>
       </c>
       <c r="Z7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AA7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AB7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AC7">
         <v>155</v>
       </c>
       <c r="AD7" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AE7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AF7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.2">
@@ -1629,22 +1629,22 @@
         <v>38</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F8">
         <v>432442342</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H8" s="5">
         <v>32787</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>42</v>
+        <v>129</v>
       </c>
       <c r="J8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K8" s="8"/>
       <c r="L8" s="7">
@@ -1654,31 +1654,31 @@
         <v>1</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="Q8" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="R8" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S8" s="10">
         <v>40271</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U8" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="V8" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="W8" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="X8">
         <v>1200000</v>
@@ -1687,25 +1687,25 @@
         <v>800000</v>
       </c>
       <c r="Z8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AA8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB8" t="s">
         <v>89</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>90</v>
       </c>
       <c r="AC8">
         <v>155</v>
       </c>
       <c r="AD8" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AE8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.2">
@@ -1728,16 +1728,16 @@
         <v>423423423</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H9" s="5">
         <v>31818</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>42</v>
+        <v>129</v>
       </c>
       <c r="J9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K9" s="8"/>
       <c r="L9" s="7">
@@ -1745,31 +1745,31 @@
       </c>
       <c r="M9" s="9"/>
       <c r="O9" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="Q9" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="R9" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S9" s="10">
         <v>40272</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U9" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V9" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="X9">
         <v>1500000</v>
@@ -1778,25 +1778,25 @@
         <v>900000</v>
       </c>
       <c r="Z9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AA9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AB9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AC9">
         <v>145</v>
       </c>
       <c r="AD9" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.2">
@@ -1813,54 +1813,54 @@
         <v>40</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F10">
         <v>423432423</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H10" s="5">
         <v>29559</v>
       </c>
       <c r="I10" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="J10" t="s">
+        <v>48</v>
+      </c>
+      <c r="K10" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="J10" t="s">
-        <v>49</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
       <c r="O10" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q10" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="Q10" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="R10" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S10" s="10">
         <v>40273</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U10" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V10" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="X10">
         <v>800000</v>
@@ -1869,25 +1869,25 @@
         <v>300000</v>
       </c>
       <c r="Z10" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA10" t="s">
         <v>86</v>
       </c>
-      <c r="AA10" t="s">
-        <v>87</v>
-      </c>
       <c r="AB10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AC10">
         <v>140</v>
       </c>
       <c r="AD10" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AE10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AF10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
adding edit identitas, riwyat to user profile page, fixing bugs
</commit_message>
<xml_diff>
--- a/public/files/formatAnggotaCu.xlsx
+++ b/public/files/formatAnggotaCu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB4507E-7446-4043-92B4-D32170F8FB0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F594BF-796B-5344-B667-B1826258D7F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{6E3E5F2B-8BA1-F845-BBF4-F30D4ACC6EF2}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{6E3E5F2B-8BA1-F845-BBF4-F30D4ACC6EF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Work Sheet" sheetId="2" r:id="rId1"/>
@@ -1481,18 +1481,25 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1509,7 +1516,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1527,6 +1534,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1890,7 +1900,7 @@
   <dimension ref="A1:AJ12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="AA13" sqref="AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1904,19 +1914,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="15" t="s">
         <v>11</v>
       </c>
       <c r="F1" s="12" t="s">
@@ -1925,19 +1935,19 @@
       <c r="G1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="K1" t="s">
         <v>2</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="13" t="s">
         <v>3</v>
       </c>
       <c r="M1" t="s">
@@ -1946,22 +1956,22 @@
       <c r="N1" t="s">
         <v>15</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="13" t="s">
         <v>18</v>
       </c>
       <c r="S1" t="s">
         <v>4</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="13" t="s">
         <v>20</v>
       </c>
       <c r="U1" t="s">
@@ -1985,10 +1995,10 @@
       <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AB1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AC1" s="13" t="s">
         <v>33</v>
       </c>
       <c r="AD1" t="s">
@@ -2015,6 +2025,7 @@
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
+      <c r="B2" s="14"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>

</xml_diff>

<commit_message>
adding auto generate nik and notification interval
</commit_message>
<xml_diff>
--- a/public/files/formatAnggotaCu.xlsx
+++ b/public/files/formatAnggotaCu.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Sites/bkcuvue/public/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F594BF-796B-5344-B667-B1826258D7F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED6FBDB-D64F-F645-A7E8-C5655AA649A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{6E3E5F2B-8BA1-F845-BBF4-F30D4ACC6EF2}"/>
   </bookViews>
@@ -240,9 +240,6 @@
     <t>rata_rata_pengeluaran_perbulan</t>
   </si>
   <si>
-    <t>alih_waris</t>
-  </si>
-  <si>
     <t>status_pernikahan</t>
   </si>
   <si>
@@ -1414,6 +1411,9 @@
   </si>
   <si>
     <t>LAINNYA</t>
+  </si>
+  <si>
+    <t>ahli_waris</t>
   </si>
 </sst>
 </file>
@@ -1899,8 +1899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B728F6F-ED4D-754B-AFD8-5624DAAEA7F5}">
   <dimension ref="A1:AJ12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="AA13" sqref="AA13"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="134" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1930,10 +1930,10 @@
         <v>11</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1" s="13" t="s">
         <v>12</v>
@@ -1984,7 +1984,7 @@
         <v>22</v>
       </c>
       <c r="X1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y1" t="s">
         <v>23</v>
@@ -1996,19 +1996,19 @@
         <v>25</v>
       </c>
       <c r="AB1" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="AC1" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF1" t="s">
         <v>27</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>28</v>
       </c>
       <c r="AG1" t="s">
         <v>7</v>
@@ -2017,10 +2017,10 @@
         <v>6</v>
       </c>
       <c r="AI1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>29</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.2">
@@ -2261,447 +2261,447 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -2724,1477 +2724,1477 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>